<commit_message>
images up to 66
</commit_message>
<xml_diff>
--- a/Comedy_Database.xlsx
+++ b/Comedy_Database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="267">
   <si>
     <t>Filename</t>
   </si>
@@ -558,6 +558,273 @@
   </si>
   <si>
     <t>harambe_bigger_2017</t>
+  </si>
+  <si>
+    <t>Unlocked</t>
+  </si>
+  <si>
+    <t>Noomi Rapace</t>
+  </si>
+  <si>
+    <t>Orlando Bloom</t>
+  </si>
+  <si>
+    <t>Toni Collette</t>
+  </si>
+  <si>
+    <t>unlocked_2017</t>
+  </si>
+  <si>
+    <t>Inception</t>
+  </si>
+  <si>
+    <t>inception_2010</t>
+  </si>
+  <si>
+    <t>Star Wars: The Force Awakens</t>
+  </si>
+  <si>
+    <t>Daisy Ridley</t>
+  </si>
+  <si>
+    <t>John Boyega</t>
+  </si>
+  <si>
+    <t>Oscar Isaac</t>
+  </si>
+  <si>
+    <t>star_wars_2015</t>
+  </si>
+  <si>
+    <t>Mad Max: Fury Road</t>
+  </si>
+  <si>
+    <t>mad_max_2015</t>
+  </si>
+  <si>
+    <t>Batman v Superman: Dawn of Justice</t>
+  </si>
+  <si>
+    <t>Henry Cavill</t>
+  </si>
+  <si>
+    <t>Amy Adams</t>
+  </si>
+  <si>
+    <t>batman_2016</t>
+  </si>
+  <si>
+    <t>Watchmen</t>
+  </si>
+  <si>
+    <t>Jackie Earle Haley</t>
+  </si>
+  <si>
+    <t>Patrick Wilson</t>
+  </si>
+  <si>
+    <t>Carla Gugino</t>
+  </si>
+  <si>
+    <t>watchmen_2009</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>avatar_2009</t>
+  </si>
+  <si>
+    <t>Jungle</t>
+  </si>
+  <si>
+    <t>Daniel Radcliffe</t>
+  </si>
+  <si>
+    <t>Thomas Kretschmann</t>
+  </si>
+  <si>
+    <t>Lily Sullivan</t>
+  </si>
+  <si>
+    <t>jungle_2017</t>
+  </si>
+  <si>
+    <t>Star Trek: Beyond</t>
+  </si>
+  <si>
+    <t>Zachary Quinto</t>
+  </si>
+  <si>
+    <t>Karl Urban</t>
+  </si>
+  <si>
+    <t>star_trek_2016</t>
+  </si>
+  <si>
+    <t>San Andreas</t>
+  </si>
+  <si>
+    <t>san_andreas_2015</t>
+  </si>
+  <si>
+    <t>Doctor Strange</t>
+  </si>
+  <si>
+    <t>Benedict Cumberbatch</t>
+  </si>
+  <si>
+    <t>Chiwetel Ejiofor</t>
+  </si>
+  <si>
+    <t>Rachel McAdams</t>
+  </si>
+  <si>
+    <t>doctor_strange_2016</t>
+  </si>
+  <si>
+    <t>Cowboys &amp; Aliens</t>
+  </si>
+  <si>
+    <t>Daniel Craig</t>
+  </si>
+  <si>
+    <t>Harrison Ford</t>
+  </si>
+  <si>
+    <t>cowboys_2011</t>
+  </si>
+  <si>
+    <t>Olivia Wilde</t>
+  </si>
+  <si>
+    <t>Allegiant</t>
+  </si>
+  <si>
+    <t>Shailene Woodley</t>
+  </si>
+  <si>
+    <t>Theo James</t>
+  </si>
+  <si>
+    <t>Jeff Daniels</t>
+  </si>
+  <si>
+    <t>allegiant_2016</t>
+  </si>
+  <si>
+    <t>Power Rangers</t>
+  </si>
+  <si>
+    <t>power_rangers_2017</t>
+  </si>
+  <si>
+    <t>The Avengers</t>
+  </si>
+  <si>
+    <t>Robert Downey Jr.</t>
+  </si>
+  <si>
+    <t>Chris Evans</t>
+  </si>
+  <si>
+    <t>avengers_2012</t>
+  </si>
+  <si>
+    <t>Jumanji</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>jumanji_1995</t>
+  </si>
+  <si>
+    <t>Transformers</t>
+  </si>
+  <si>
+    <t>transformers_2007</t>
+  </si>
+  <si>
+    <t>Maze Runner: The Scorch Trials</t>
+  </si>
+  <si>
+    <t>maze_runner_2015</t>
+  </si>
+  <si>
+    <t>Spectre</t>
+  </si>
+  <si>
+    <t>Christoph Waltz</t>
+  </si>
+  <si>
+    <t>Léa Seydoux</t>
+  </si>
+  <si>
+    <t>spectre_2015</t>
+  </si>
+  <si>
+    <t>Sicario</t>
+  </si>
+  <si>
+    <t>Emily Blunt</t>
+  </si>
+  <si>
+    <t>Josh Brolin</t>
+  </si>
+  <si>
+    <t>Benicio Del Toro</t>
+  </si>
+  <si>
+    <t>sicario_2015</t>
+  </si>
+  <si>
+    <t>John Wick</t>
+  </si>
+  <si>
+    <t>Michael Nyqvist</t>
+  </si>
+  <si>
+    <t>Alfie Allen</t>
+  </si>
+  <si>
+    <t>john_wick_2014</t>
+  </si>
+  <si>
+    <t>The Dark Knight Rises</t>
+  </si>
+  <si>
+    <t>the_dark_knight_2012</t>
+  </si>
+  <si>
+    <t>Captain America: Civil War</t>
+  </si>
+  <si>
+    <t>captain_america_2016</t>
+  </si>
+  <si>
+    <t>X-Men: Apocalypse</t>
+  </si>
+  <si>
+    <t>Jennifer Lawrence </t>
+  </si>
+  <si>
+    <t>xmen_2016</t>
+  </si>
+  <si>
+    <t>Tombstone</t>
+  </si>
+  <si>
+    <t>Kurt Russell</t>
+  </si>
+  <si>
+    <t>Val Kilmer</t>
+  </si>
+  <si>
+    <t>Sam Elliott</t>
+  </si>
+  <si>
+    <t>tombstone_1993</t>
   </si>
 </sst>
 </file>
@@ -593,8 +860,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,8 +1180,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,196 +2449,871 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42">
+        <v>2017</v>
+      </c>
       <c r="D42" t="s">
         <v>32</v>
       </c>
+      <c r="E42" t="s">
+        <v>66</v>
+      </c>
+      <c r="F42" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42">
+        <v>6.1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>179</v>
+      </c>
+      <c r="J42" t="s">
+        <v>180</v>
+      </c>
+      <c r="K42" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C43">
+        <v>2010</v>
+      </c>
       <c r="D43" t="s">
         <v>32</v>
       </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44">
+        <v>2015</v>
+      </c>
       <c r="D44" t="s">
         <v>32</v>
       </c>
+      <c r="E44" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44">
+        <v>8.1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>186</v>
+      </c>
+      <c r="J44" t="s">
+        <v>187</v>
+      </c>
+      <c r="K44" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" t="s">
+        <v>190</v>
+      </c>
+      <c r="C45">
+        <v>2015</v>
+      </c>
       <c r="D45" t="s">
         <v>32</v>
       </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>53</v>
+      </c>
+      <c r="G45">
+        <v>8.1</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46" t="s">
+        <v>192</v>
+      </c>
+      <c r="C46">
+        <v>2016</v>
+      </c>
       <c r="D46" t="s">
         <v>32</v>
       </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46">
+        <v>6.6</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46" t="s">
+        <v>137</v>
+      </c>
+      <c r="J46" t="s">
+        <v>193</v>
+      </c>
+      <c r="K46" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>200</v>
+      </c>
+      <c r="B47" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47">
+        <v>2009</v>
+      </c>
       <c r="D47" t="s">
         <v>32</v>
       </c>
+      <c r="E47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" t="s">
+        <v>119</v>
+      </c>
+      <c r="G47">
+        <v>7.6</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>197</v>
+      </c>
+      <c r="J47" t="s">
+        <v>198</v>
+      </c>
+      <c r="K47" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>202</v>
+      </c>
+      <c r="B48" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48">
+        <v>2009</v>
+      </c>
       <c r="D48" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48">
+        <v>7.8</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49">
+        <v>2017</v>
+      </c>
       <c r="D49" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49">
+        <v>7.2</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>204</v>
+      </c>
+      <c r="J49" t="s">
+        <v>205</v>
+      </c>
+      <c r="K49" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C50">
+        <v>2016</v>
+      </c>
       <c r="D50" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G50">
+        <v>7.1</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>35</v>
+      </c>
+      <c r="J50" t="s">
+        <v>209</v>
+      </c>
+      <c r="K50" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>213</v>
+      </c>
+      <c r="B51" t="s">
+        <v>212</v>
+      </c>
+      <c r="C51">
+        <v>2015</v>
+      </c>
       <c r="D51" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51">
+        <v>6.1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>82</v>
+      </c>
+      <c r="J51" t="s">
+        <v>199</v>
+      </c>
+      <c r="K51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>218</v>
+      </c>
+      <c r="B52" t="s">
+        <v>214</v>
+      </c>
+      <c r="C52">
+        <v>2016</v>
+      </c>
       <c r="D52" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" t="s">
+        <v>33</v>
+      </c>
+      <c r="G52">
+        <v>7.5</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>215</v>
+      </c>
+      <c r="J52" t="s">
+        <v>216</v>
+      </c>
+      <c r="K52" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" t="s">
+        <v>219</v>
+      </c>
+      <c r="C53">
+        <v>2011</v>
+      </c>
       <c r="D53" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>43</v>
+      </c>
+      <c r="G53">
+        <v>6</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
+        <v>220</v>
+      </c>
+      <c r="J53" t="s">
+        <v>221</v>
+      </c>
+      <c r="K53" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>228</v>
+      </c>
+      <c r="B54" t="s">
+        <v>224</v>
+      </c>
+      <c r="C54">
+        <v>2016</v>
+      </c>
       <c r="D54" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" t="s">
+        <v>119</v>
+      </c>
+      <c r="G54">
+        <v>5.7</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54" t="s">
+        <v>225</v>
+      </c>
+      <c r="J54" t="s">
+        <v>226</v>
+      </c>
+      <c r="K54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>230</v>
+      </c>
+      <c r="B55" t="s">
+        <v>229</v>
+      </c>
+      <c r="C55">
+        <v>2017</v>
+      </c>
       <c r="D55" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" t="s">
+        <v>53</v>
+      </c>
+      <c r="G55">
+        <v>6.1</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>234</v>
+      </c>
+      <c r="B56" t="s">
+        <v>231</v>
+      </c>
+      <c r="C56">
+        <v>2012</v>
+      </c>
       <c r="D56" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" t="s">
+        <v>53</v>
+      </c>
+      <c r="G56">
+        <v>8.1</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>232</v>
+      </c>
+      <c r="J56" t="s">
+        <v>233</v>
+      </c>
+      <c r="K56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>237</v>
+      </c>
+      <c r="B57" t="s">
+        <v>235</v>
+      </c>
+      <c r="C57">
+        <v>1995</v>
+      </c>
       <c r="D57" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" t="s">
+        <v>236</v>
+      </c>
+      <c r="G57">
+        <v>6.9</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>239</v>
+      </c>
+      <c r="B58" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58">
+        <v>2007</v>
+      </c>
       <c r="D58" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G58">
+        <v>7.1</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>241</v>
+      </c>
+      <c r="B59" t="s">
+        <v>240</v>
+      </c>
+      <c r="C59">
+        <v>2015</v>
+      </c>
       <c r="D59" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" t="s">
+        <v>43</v>
+      </c>
+      <c r="G59">
+        <v>6.3</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>245</v>
+      </c>
+      <c r="B60" t="s">
+        <v>242</v>
+      </c>
+      <c r="C60">
+        <v>2015</v>
+      </c>
       <c r="D60" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F60" t="s">
+        <v>43</v>
+      </c>
+      <c r="G60">
+        <v>6.8</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60" t="s">
+        <v>220</v>
+      </c>
+      <c r="J60" t="s">
+        <v>243</v>
+      </c>
+      <c r="K60" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>250</v>
+      </c>
+      <c r="B61" t="s">
+        <v>246</v>
+      </c>
+      <c r="C61">
+        <v>2015</v>
+      </c>
       <c r="D61" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" t="s">
+        <v>66</v>
+      </c>
+      <c r="G61">
+        <v>7.6</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
+        <v>247</v>
+      </c>
+      <c r="J61" t="s">
+        <v>248</v>
+      </c>
+      <c r="K61" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>254</v>
+      </c>
+      <c r="B62" t="s">
+        <v>251</v>
+      </c>
+      <c r="C62">
+        <v>2014</v>
+      </c>
       <c r="D62" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" t="s">
+        <v>43</v>
+      </c>
+      <c r="G62">
+        <v>7.3</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62" t="s">
+        <v>165</v>
+      </c>
+      <c r="J62" t="s">
+        <v>252</v>
+      </c>
+      <c r="K62" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>256</v>
+      </c>
+      <c r="B63" t="s">
+        <v>255</v>
+      </c>
+      <c r="C63">
+        <v>2012</v>
+      </c>
       <c r="D63" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>43</v>
+      </c>
+      <c r="G63">
+        <v>8.4</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>258</v>
+      </c>
+      <c r="B64" t="s">
+        <v>257</v>
+      </c>
+      <c r="C64">
+        <v>2016</v>
+      </c>
       <c r="D64" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>21</v>
+      </c>
+      <c r="F64" t="s">
+        <v>53</v>
+      </c>
+      <c r="G64">
+        <v>7.9</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>233</v>
+      </c>
+      <c r="J64" t="s">
+        <v>232</v>
+      </c>
+      <c r="K64" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" t="s">
+        <v>259</v>
+      </c>
+      <c r="C65">
+        <v>2016</v>
+      </c>
       <c r="D65" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>21</v>
+      </c>
+      <c r="F65" t="s">
+        <v>53</v>
+      </c>
+      <c r="G65">
+        <v>7</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>121</v>
+      </c>
+      <c r="J65" t="s">
+        <v>87</v>
+      </c>
+      <c r="K65" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>266</v>
+      </c>
+      <c r="B66" t="s">
+        <v>262</v>
+      </c>
+      <c r="C66">
+        <v>1993</v>
+      </c>
       <c r="D66" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" t="s">
+        <v>66</v>
+      </c>
+      <c r="G66">
+        <v>7.8</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66" t="s">
+        <v>263</v>
+      </c>
+      <c r="J66" t="s">
+        <v>264</v>
+      </c>
+      <c r="K66" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
         <v>32</v>
       </c>

</xml_diff>